<commit_message>
Last version 9:05 am. I have problems with server, and I decided to work since my computer
</commit_message>
<xml_diff>
--- a/06_Statistical_Preparation/KFactors_by_coupling/wRHC/tau_tau.xlsx
+++ b/06_Statistical_Preparation/KFactors_by_coupling/wRHC/tau_tau.xlsx
@@ -461,25 +461,25 @@
         <v>0.25</v>
       </c>
       <c r="B2" t="n">
-        <v>0.003981456953642384</v>
+        <v>0.0003933774834437086</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0105900430239705</v>
+        <v>0.0003915181315304241</v>
       </c>
       <c r="D2" t="n">
-        <v>0.02195606305076331</v>
+        <v>0.0003985354350254437</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0399909008189263</v>
+        <v>0.0004071883530482257</v>
       </c>
       <c r="F2" t="n">
-        <v>0.06029298380878952</v>
+        <v>0.0004163454124903623</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1065060240963855</v>
+        <v>0.0004096987951807229</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1665457842248413</v>
+        <v>0.0004116953762466002</v>
       </c>
     </row>
     <row r="3">
@@ -487,25 +487,25 @@
         <v>0.5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.007520529801324503</v>
+        <v>0.006193377483443708</v>
       </c>
       <c r="C3" t="n">
-        <v>0.01194837123540258</v>
+        <v>0.006306084818684696</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01759960282983741</v>
+        <v>0.006228124612138513</v>
       </c>
       <c r="E3" t="n">
-        <v>0.03093721565059145</v>
+        <v>0.006528662420382165</v>
       </c>
       <c r="F3" t="n">
-        <v>0.05917501927525057</v>
+        <v>0.006626831148804934</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1019277108433735</v>
+        <v>0.006656626506024096</v>
       </c>
       <c r="H3" t="n">
-        <v>0.141976427923844</v>
+        <v>0.006533998186763373</v>
       </c>
     </row>
     <row r="4">
@@ -513,25 +513,25 @@
         <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>0.08585430463576159</v>
+        <v>0.09928476821192053</v>
       </c>
       <c r="C4" t="n">
-        <v>0.09004302397049783</v>
+        <v>0.1011063306699447</v>
       </c>
       <c r="D4" t="n">
-        <v>0.09415415166935584</v>
+        <v>0.1022961400024823</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1033666969972703</v>
+        <v>0.1044358507734304</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1216653816499614</v>
+        <v>0.1058596761757903</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1491566265060241</v>
+        <v>0.1031927710843373</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1880326382592928</v>
+        <v>0.1058930190389846</v>
       </c>
     </row>
     <row r="5">
@@ -539,25 +539,25 @@
         <v>1.5</v>
       </c>
       <c r="B5" t="n">
-        <v>0.4789403973509934</v>
+        <v>0.4998675496688742</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4482483097725875</v>
+        <v>0.5144437615242777</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4733771875387862</v>
+        <v>0.5150800546108973</v>
       </c>
       <c r="E5" t="n">
-        <v>0.4813466787989081</v>
+        <v>0.5286624203821656</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4826522744795682</v>
+        <v>0.5366229760986893</v>
       </c>
       <c r="G5" t="n">
-        <v>0.4864457831325302</v>
+        <v>0.5283734939759036</v>
       </c>
       <c r="H5" t="n">
-        <v>0.51532184950136</v>
+        <v>0.5332728921124207</v>
       </c>
     </row>
     <row r="6">
@@ -591,25 +591,25 @@
         <v>2</v>
       </c>
       <c r="B7" t="n">
-        <v>1.543311258278146</v>
+        <v>1.587019867549669</v>
       </c>
       <c r="C7" t="n">
-        <v>1.518131530424093</v>
+        <v>1.606023355869699</v>
       </c>
       <c r="D7" t="n">
-        <v>1.557651731413678</v>
+        <v>1.645773861238674</v>
       </c>
       <c r="E7" t="n">
-        <v>1.544813466787989</v>
+        <v>1.669699727024568</v>
       </c>
       <c r="F7" t="n">
-        <v>1.553199691595991</v>
+        <v>1.69313801079414</v>
       </c>
       <c r="G7" t="n">
-        <v>1.51566265060241</v>
+        <v>1.676506024096386</v>
       </c>
       <c r="H7" t="n">
-        <v>1.501359927470535</v>
+        <v>1.694469628286491</v>
       </c>
     </row>
     <row r="8">
@@ -617,25 +617,25 @@
         <v>2.5</v>
       </c>
       <c r="B8" t="n">
-        <v>3.790728476821192</v>
+        <v>3.856953642384106</v>
       </c>
       <c r="C8" t="n">
-        <v>3.547633681622618</v>
+        <v>3.884449907805777</v>
       </c>
       <c r="D8" t="n">
-        <v>3.821521658185429</v>
+        <v>4.00893632865831</v>
       </c>
       <c r="E8" t="n">
-        <v>3.839854413102821</v>
+        <v>4.076433121019108</v>
       </c>
       <c r="F8" t="n">
-        <v>3.87047031611411</v>
+        <v>4.117193523515806</v>
       </c>
       <c r="G8" t="n">
-        <v>3.730722891566265</v>
+        <v>4.119879518072289</v>
       </c>
       <c r="H8" t="n">
-        <v>3.690843155031732</v>
+        <v>4.115140525838622</v>
       </c>
     </row>
     <row r="9">
@@ -643,25 +643,25 @@
         <v>3</v>
       </c>
       <c r="B9" t="n">
-        <v>7.84635761589404</v>
+        <v>8.055629139072847</v>
       </c>
       <c r="C9" t="n">
-        <v>8.027043638598647</v>
+        <v>8.168408113091578</v>
       </c>
       <c r="D9" t="n">
-        <v>8.001737619461338</v>
+        <v>8.321956063050763</v>
       </c>
       <c r="E9" t="n">
-        <v>8.105095541401274</v>
+        <v>8.47361237488626</v>
       </c>
       <c r="F9" t="n">
-        <v>8.191981495759444</v>
+        <v>8.600616808018504</v>
       </c>
       <c r="G9" t="n">
-        <v>8.03012048192771</v>
+        <v>8.445783132530121</v>
       </c>
       <c r="H9" t="n">
-        <v>7.820489573889393</v>
+        <v>8.556663644605621</v>
       </c>
     </row>
     <row r="10">
@@ -669,25 +669,25 @@
         <v>3.5</v>
       </c>
       <c r="B10" t="n">
-        <v>14.28079470198676</v>
+        <v>14.25960264900662</v>
       </c>
       <c r="C10" t="n">
-        <v>14.81253841425937</v>
+        <v>15.09526736324523</v>
       </c>
       <c r="D10" t="n">
-        <v>14.99317363783046</v>
+        <v>15.41516693558396</v>
       </c>
       <c r="E10" t="n">
-        <v>15.20018198362147</v>
+        <v>15.7393084622384</v>
       </c>
       <c r="F10" t="n">
-        <v>15.09252120277564</v>
+        <v>15.7710100231303</v>
       </c>
       <c r="G10" t="n">
-        <v>15.10240963855422</v>
+        <v>15.7289156626506</v>
       </c>
       <c r="H10" t="n">
-        <v>14.95013599274705</v>
+        <v>15.90208522212149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>